<commit_message>
Updates to Data and Affects
</commit_message>
<xml_diff>
--- a/Server/testData/rawAffects/NewAffects.xlsx
+++ b/Server/testData/rawAffects/NewAffects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming-School\eec-common-repo\Server\testData\rawAffects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480F9AA9-3953-48B1-8AC1-345E58ADA845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74CD641-5F50-486A-9CEF-9E7E6F0482F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21885" yWindow="1080" windowWidth="27870" windowHeight="18690" xr2:uid="{29D9A252-B3D8-4ABB-AC96-716C0C40817A}"/>
   </bookViews>
@@ -54,15 +54,6 @@
     <t>Star-Struck</t>
   </si>
   <si>
-    <t>Anxious Face w Sweat</t>
-  </si>
-  <si>
-    <t>Grinning Face w Smiling Eyes</t>
-  </si>
-  <si>
-    <t>Face w Steam From Nose</t>
-  </si>
-  <si>
     <t>Grinning Squinting Face</t>
   </si>
   <si>
@@ -81,18 +72,9 @@
     <t>Confused Face</t>
   </si>
   <si>
-    <t>Beaming Face w Smiling Eyes</t>
-  </si>
-  <si>
     <t>Yawning Face</t>
   </si>
   <si>
-    <t>Grinning Face w Big Eyes</t>
-  </si>
-  <si>
-    <t>Downcast Face w Sweat</t>
-  </si>
-  <si>
     <t>Partying Face</t>
   </si>
   <si>
@@ -105,9 +87,6 @@
     <t>Sleepy Face</t>
   </si>
   <si>
-    <t>Smiling Face w Halo</t>
-  </si>
-  <si>
     <t>Disappointed Face</t>
   </si>
   <si>
@@ -349,6 +328,27 @@
   </si>
   <si>
     <t>☺️</t>
+  </si>
+  <si>
+    <t>Beaming Face with Smiling Eyes</t>
+  </si>
+  <si>
+    <t>Grinning Face with Big Eyes</t>
+  </si>
+  <si>
+    <t>Grinning Face with Smiling Eyes</t>
+  </si>
+  <si>
+    <t>Smiling Face with Halo</t>
+  </si>
+  <si>
+    <t>Downcast Face with Sweat</t>
+  </si>
+  <si>
+    <t>Face with Steam From Nose</t>
+  </si>
+  <si>
+    <t>Anxious Face with Sweat</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:U26"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,16 +776,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -794,24 +794,24 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J2" t="str">
         <f xml:space="preserve"> "{ "</f>
@@ -846,7 +846,7 @@
         <v/>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -857,27 +857,27 @@
         <v>"active": true</v>
       </c>
       <c r="U2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J25" si="0" xml:space="preserve"> "{ "</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="L3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Beaming Face w Smiling Eyes",</v>
+        <v>"description": "Beaming Face with Smiling Eyes",</v>
       </c>
       <c r="M3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -912,7 +912,7 @@
         <v/>
       </c>
       <c r="R3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -923,30 +923,30 @@
         <v>"active": true</v>
       </c>
       <c r="U3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
@@ -981,7 +981,7 @@
         <v/>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -992,24 +992,24 @@
         <v>"active": true</v>
       </c>
       <c r="U4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="L5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grinning Face w Big Eyes",</v>
+        <v>"description": "Grinning Face with Big Eyes",</v>
       </c>
       <c r="M5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -1044,7 +1044,7 @@
         <v/>
       </c>
       <c r="R5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1055,30 +1055,30 @@
         <v>"active": true</v>
       </c>
       <c r="U5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="L6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grinning Face w Smiling Eyes",</v>
+        <v>"description": "Grinning Face with Smiling Eyes",</v>
       </c>
       <c r="M6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -1113,7 +1113,7 @@
         <v/>
       </c>
       <c r="R6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1124,27 +1124,27 @@
         <v>"active": true</v>
       </c>
       <c r="U6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -1179,7 +1179,7 @@
         <v/>
       </c>
       <c r="R7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1190,27 +1190,27 @@
         <v>"active": true</v>
       </c>
       <c r="U7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="L8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Smiling Face w Halo",</v>
+        <v>"description": "Smiling Face with Halo",</v>
       </c>
       <c r="M8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -1245,7 +1245,7 @@
         <v/>
       </c>
       <c r="R8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1256,27 +1256,27 @@
         <v>"active": true</v>
       </c>
       <c r="U8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -1311,7 +1311,7 @@
         <v/>
       </c>
       <c r="R9" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1322,24 +1322,24 @@
         <v>"active": true</v>
       </c>
       <c r="U9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -1374,7 +1374,7 @@
         <v/>
       </c>
       <c r="R10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1385,30 +1385,30 @@
         <v>"active": true</v>
       </c>
       <c r="U10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -1443,7 +1443,7 @@
         <v/>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1454,24 +1454,24 @@
         <v>"active": true</v>
       </c>
       <c r="U11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G12" s="1">
         <v>-1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -1506,7 +1506,7 @@
         <v/>
       </c>
       <c r="R12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1517,24 +1517,24 @@
         <v>"active": true</v>
       </c>
       <c r="U12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G13" s="1">
         <v>-1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="L13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Downcast Face w Sweat",</v>
+        <v>"description": "Downcast Face with Sweat",</v>
       </c>
       <c r="M13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -1569,7 +1569,7 @@
         <v/>
       </c>
       <c r="R13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1580,24 +1580,24 @@
         <v>"active": true</v>
       </c>
       <c r="U13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -1632,7 +1632,7 @@
         <v/>
       </c>
       <c r="R14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1643,27 +1643,27 @@
         <v>"active": true</v>
       </c>
       <c r="U14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G15" s="1">
         <v>-1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -1698,7 +1698,7 @@
         <v/>
       </c>
       <c r="R15" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1709,27 +1709,27 @@
         <v>"active": true</v>
       </c>
       <c r="U15" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G16" s="1">
         <v>-1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -1764,7 +1764,7 @@
         <v/>
       </c>
       <c r="R16" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1775,27 +1775,27 @@
         <v>"active": true</v>
       </c>
       <c r="U16" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G17" s="1">
         <v>-1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -1830,7 +1830,7 @@
         <v/>
       </c>
       <c r="R17" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1841,24 +1841,24 @@
         <v>"active": true</v>
       </c>
       <c r="U17" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G18" s="1">
         <v>-1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="L18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Face w Steam From Nose",</v>
+        <v>"description": "Face with Steam From Nose",</v>
       </c>
       <c r="M18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -1893,7 +1893,7 @@
         <v/>
       </c>
       <c r="R18" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1904,24 +1904,24 @@
         <v>"active": true</v>
       </c>
       <c r="U18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -1956,7 +1956,7 @@
         <v/>
       </c>
       <c r="R19" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1967,27 +1967,27 @@
         <v>"active": true</v>
       </c>
       <c r="U19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G20" s="1">
         <v>-1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -2022,7 +2022,7 @@
         <v/>
       </c>
       <c r="R20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2033,27 +2033,27 @@
         <v>"active": true</v>
       </c>
       <c r="U20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1">
         <v>-1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="L21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Anxious Face w Sweat",</v>
+        <v>"description": "Anxious Face with Sweat",</v>
       </c>
       <c r="M21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
@@ -2088,7 +2088,7 @@
         <v/>
       </c>
       <c r="R21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2099,30 +2099,30 @@
         <v>"active": true</v>
       </c>
       <c r="U21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -2157,7 +2157,7 @@
         <v/>
       </c>
       <c r="R22" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2168,33 +2168,33 @@
         <v>"active": true</v>
       </c>
       <c r="U22" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -2229,7 +2229,7 @@
         <v>"Amazement"</v>
       </c>
       <c r="R23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2240,24 +2240,24 @@
         <v>"active": true</v>
       </c>
       <c r="U23" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G24" s="1">
         <v>-1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -2292,7 +2292,7 @@
         <v/>
       </c>
       <c r="R24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2303,24 +2303,24 @@
         <v>"active": true</v>
       </c>
       <c r="U24" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -2355,7 +2355,7 @@
         <v/>
       </c>
       <c r="R25" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2366,12 +2366,12 @@
         <v>"active": true</v>
       </c>
       <c r="U25" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some emoji/affect bugs
</commit_message>
<xml_diff>
--- a/Server/testData/rawAffects/NewAffects.xlsx
+++ b/Server/testData/rawAffects/NewAffects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming-School\eec-common-repo\Server\testData\rawAffects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berriers/Programming/eec-common-repo/Server/testData/rawAffects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74CD641-5F50-486A-9CEF-9E7E6F0482F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970250E-15A0-5242-9204-EDF460D012FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21885" yWindow="1080" windowWidth="27870" windowHeight="18690" xr2:uid="{29D9A252-B3D8-4ABB-AC96-716C0C40817A}"/>
+    <workbookView xWindow="-40940" yWindow="2660" windowWidth="40960" windowHeight="22540" xr2:uid="{29D9A252-B3D8-4ABB-AC96-716C0C40817A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="119">
   <si>
     <t>name</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Worried Face</t>
   </si>
   <si>
-    <t>Smiling Face</t>
-  </si>
-  <si>
     <t>Smirking Face</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>Disappointment</t>
   </si>
   <si>
-    <t>☺️</t>
-  </si>
-  <si>
     <t>Beaming Face with Smiling Eyes</t>
   </si>
   <si>
@@ -349,6 +343,54 @@
   </si>
   <si>
     <t>Anxious Face with Sweat</t>
+  </si>
+  <si>
+    <t>😎</t>
+  </si>
+  <si>
+    <t>Ambivalent, Neutral</t>
+  </si>
+  <si>
+    <t>😐</t>
+  </si>
+  <si>
+    <t>Smiling Face with Sunglasses</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>Energized</t>
+  </si>
+  <si>
+    <t>Uninterested</t>
+  </si>
+  <si>
+    <t>Celebrate</t>
+  </si>
+  <si>
+    <t>Congrats</t>
+  </si>
+  <si>
+    <t>Congratulations</t>
+  </si>
+  <si>
+    <t>Exhausted</t>
+  </si>
+  <si>
+    <t>Exhaustion</t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>Confusion</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Face with Straight Mouth</t>
   </si>
 </sst>
 </file>
@@ -396,7 +438,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -420,20 +471,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97209CC2-D696-43B9-8172-723D835F28A1}" name="Table1" displayName="Table1" ref="A1:H25" totalsRowShown="0">
-  <autoFilter ref="A1:H25" xr:uid="{97209CC2-D696-43B9-8172-723D835F28A1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H25">
-    <sortCondition ref="C1:C25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97209CC2-D696-43B9-8172-723D835F28A1}" name="Table1" displayName="Table1" ref="A1:H27" totalsRowCount="1">
+  <autoFilter ref="A1:H26" xr:uid="{97209CC2-D696-43B9-8172-723D835F28A1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H26">
+    <sortCondition ref="C1:C26"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{937E03AA-42B8-4F21-8CED-841BB10CDD05}" name="name"/>
+    <tableColumn id="1" xr3:uid="{937E03AA-42B8-4F21-8CED-841BB10CDD05}" name="name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F560CCD9-0FE5-4B5D-8A1D-D0BC3D9FA4E4}" name="description"/>
-    <tableColumn id="3" xr3:uid="{D1F9F36A-4F9F-43B8-B427-C52F36F043CC}" name="characterCodes" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D1F9F36A-4F9F-43B8-B427-C52F36F043CC}" name="characterCodes" dataDxfId="5" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{744D4406-D359-409C-8C64-155246DB37C4}" name="related"/>
     <tableColumn id="8" xr3:uid="{E58DFCE5-051E-4701-B194-FEEABBB3FBC5}" name="related2"/>
     <tableColumn id="7" xr3:uid="{231F6072-1022-47BD-811D-E33DB8FEE891}" name="related3"/>
-    <tableColumn id="5" xr3:uid="{FB2190ED-A4F5-4603-A60F-8C9354525546}" name="positivity" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C044B12F-37E2-408D-A1AF-524B258708DA}" name="active" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{FB2190ED-A4F5-4603-A60F-8C9354525546}" name="positivity" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C044B12F-37E2-408D-A1AF-524B258708DA}" name="active" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,39 +787,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D97DDA4-38D3-4E77-A731-071409A8387D}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,16 +827,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -794,24 +845,33 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" t="str">
         <f xml:space="preserve"> "{ "</f>
@@ -819,15 +879,15 @@
       </c>
       <c r="K2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Rested, Restored",</v>
+        <v>"name": "Admiration",</v>
       </c>
       <c r="L2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Smiling Face",</v>
+        <v>"description": "Star-Struck",</v>
       </c>
       <c r="M2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["☺️"] ,</v>
+        <v>"characterCodes": ["🤩"] ,</v>
       </c>
       <c r="N2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -835,18 +895,18 @@
       </c>
       <c r="O2" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Impressed",</v>
       </c>
       <c r="P2" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Pride",</v>
       </c>
       <c r="Q2" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
-        <v/>
+        <v>"Amazement"</v>
       </c>
       <c r="R2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S2" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -857,43 +917,43 @@
         <v>"active": true</v>
       </c>
       <c r="U2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J25" si="0" xml:space="preserve"> "{ "</f>
+        <f t="shared" ref="J3:J26" si="0" xml:space="preserve"> "{ "</f>
         <v xml:space="preserve">{ </v>
       </c>
       <c r="K3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Confident, Empowered",</v>
+        <v>"name": "Bored, Detached",</v>
       </c>
       <c r="L3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Beaming Face with Smiling Eyes",</v>
+        <v>"description": "Yawning Face",</v>
       </c>
       <c r="M3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😁"] ,</v>
+        <v>"characterCodes": ["🥱"] ,</v>
       </c>
       <c r="N3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -901,7 +961,7 @@
       </c>
       <c r="O3" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Pride"</v>
+        <v>"Uninterested"</v>
       </c>
       <c r="P3" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -912,41 +972,44 @@
         <v/>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 1,</v>
+        <v>"positivity": -1,</v>
       </c>
       <c r="T3" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>112</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
@@ -954,15 +1017,15 @@
       </c>
       <c r="K4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Joyful, Amused",</v>
+        <v>"name": "Grateful, Thankful",</v>
       </c>
       <c r="L4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Face with Tears of Joy",</v>
+        <v>"description": "Partying Face",</v>
       </c>
       <c r="M4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😂"] ,</v>
+        <v>"characterCodes": ["🥳"] ,</v>
       </c>
       <c r="N4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -970,18 +1033,18 @@
       </c>
       <c r="O4" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Happiness",</v>
+        <v>"Celebrate",</v>
       </c>
       <c r="P4" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v>"Happy"</v>
+        <v>"Congrats",</v>
       </c>
       <c r="Q4" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
-        <v/>
+        <v>"Congratulations"</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S4" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -992,24 +1055,27 @@
         <v>"active": true</v>
       </c>
       <c r="U4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -1017,15 +1083,15 @@
       </c>
       <c r="K5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Friendly, Empathetic",</v>
+        <v>"name": "Confident, Empowered",</v>
       </c>
       <c r="L5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grinning Face with Big Eyes",</v>
+        <v>"description": "Beaming Face with Smiling Eyes",</v>
       </c>
       <c r="M5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😃"] ,</v>
+        <v>"characterCodes": ["😁"] ,</v>
       </c>
       <c r="N5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1033,7 +1099,7 @@
       </c>
       <c r="O5" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Pride"</v>
       </c>
       <c r="P5" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1044,7 +1110,7 @@
         <v/>
       </c>
       <c r="R5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S5" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1055,30 +1121,30 @@
         <v>"active": true</v>
       </c>
       <c r="U5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -1086,15 +1152,15 @@
       </c>
       <c r="K6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Humor",</v>
+        <v>"name": "Joyful, Amused",</v>
       </c>
       <c r="L6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grinning Face with Smiling Eyes",</v>
+        <v>"description": "Face with Tears of Joy",</v>
       </c>
       <c r="M6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😄"] ,</v>
+        <v>"characterCodes": ["😂"] ,</v>
       </c>
       <c r="N6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1102,18 +1168,18 @@
       </c>
       <c r="O6" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Amusement",</v>
+        <v>"Happiness",</v>
       </c>
       <c r="P6" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v>"Laughter"</v>
+        <v>"Happy"</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S6" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1124,27 +1190,24 @@
         <v>"active": true</v>
       </c>
       <c r="U6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -1152,15 +1215,15 @@
       </c>
       <c r="K7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Excited, Enthusiastic",</v>
+        <v>"name": "Friendly, Empathetic",</v>
       </c>
       <c r="L7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grinning Squinting Face",</v>
+        <v>"description": "Grinning Face with Big Eyes",</v>
       </c>
       <c r="M7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😆"] ,</v>
+        <v>"characterCodes": ["😃"] ,</v>
       </c>
       <c r="N7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1168,7 +1231,7 @@
       </c>
       <c r="O7" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Awe"</v>
+        <v/>
       </c>
       <c r="P7" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1179,7 +1242,7 @@
         <v/>
       </c>
       <c r="R7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S7" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1190,27 +1253,30 @@
         <v>"active": true</v>
       </c>
       <c r="U7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
@@ -1218,15 +1284,15 @@
       </c>
       <c r="K8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Inspired",</v>
+        <v>"name": "Humor",</v>
       </c>
       <c r="L8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Smiling Face with Halo",</v>
+        <v>"description": "Grinning Face with Smiling Eyes",</v>
       </c>
       <c r="M8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😇"] ,</v>
+        <v>"characterCodes": ["😄"] ,</v>
       </c>
       <c r="N8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1234,18 +1300,18 @@
       </c>
       <c r="O8" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Idea"</v>
+        <v>"Amusement",</v>
       </c>
       <c r="P8" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Laughter"</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S8" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1256,27 +1322,27 @@
         <v>"active": true</v>
       </c>
       <c r="U8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -1284,15 +1350,15 @@
       </c>
       <c r="K9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Hopeful",</v>
+        <v>"name": "Excited, Enthusiastic",</v>
       </c>
       <c r="L9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Smiling face with Smiling Eyes",</v>
+        <v>"description": "Grinning Squinting Face",</v>
       </c>
       <c r="M9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😊"] ,</v>
+        <v>"characterCodes": ["😆"] ,</v>
       </c>
       <c r="N9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1300,7 +1366,7 @@
       </c>
       <c r="O9" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Encouraged"</v>
+        <v>"Awe"</v>
       </c>
       <c r="P9" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1311,7 +1377,7 @@
         <v/>
       </c>
       <c r="R9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S9" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1322,24 +1388,27 @@
         <v>"active": true</v>
       </c>
       <c r="U9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -1347,15 +1416,15 @@
       </c>
       <c r="K10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Relief",</v>
+        <v>"name": "Inspired",</v>
       </c>
       <c r="L10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Relieved Face",</v>
+        <v>"description": "Smiling Face with Halo",</v>
       </c>
       <c r="M10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😌"] ,</v>
+        <v>"characterCodes": ["😇"] ,</v>
       </c>
       <c r="N10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1363,7 +1432,7 @@
       </c>
       <c r="O10" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Idea"</v>
       </c>
       <c r="P10" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1374,7 +1443,7 @@
         <v/>
       </c>
       <c r="R10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S10" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1385,30 +1454,27 @@
         <v>"active": true</v>
       </c>
       <c r="U10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -1416,15 +1482,15 @@
       </c>
       <c r="K11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Jealous",</v>
+        <v>"name": "Hopeful",</v>
       </c>
       <c r="L11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Smirking Face",</v>
+        <v>"description": "Smiling face with Smiling Eyes",</v>
       </c>
       <c r="M11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😏"] ,</v>
+        <v>"characterCodes": ["😊"] ,</v>
       </c>
       <c r="N11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1432,46 +1498,46 @@
       </c>
       <c r="O11" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Envy",</v>
+        <v>"Encouraged"</v>
       </c>
       <c r="P11" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v>"Envious"</v>
+        <v/>
       </c>
       <c r="Q11" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 0,</v>
+        <v>"positivity": 1,</v>
       </c>
       <c r="T11" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -1479,15 +1545,15 @@
       </c>
       <c r="K12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Aversion, Disgust",</v>
+        <v>"name": "Relief",</v>
       </c>
       <c r="L12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Unamused Face",</v>
+        <v>"description": "Relieved Face",</v>
       </c>
       <c r="M12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😒"] ,</v>
+        <v>"characterCodes": ["😌"] ,</v>
       </c>
       <c r="N12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1506,35 +1572,41 @@
         <v/>
       </c>
       <c r="R12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": -1,</v>
+        <v>"positivity": 1,</v>
       </c>
       <c r="T12" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
+        <v>108</v>
       </c>
       <c r="G13" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -1542,15 +1614,15 @@
       </c>
       <c r="K13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Restless, Upset",</v>
+        <v>"name": "Rested, Restored",</v>
       </c>
       <c r="L13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Downcast Face with Sweat",</v>
+        <v>"description": "Smiling Face with Sunglasses",</v>
       </c>
       <c r="M13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😓"] ,</v>
+        <v>"characterCodes": ["😎"] ,</v>
       </c>
       <c r="N13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1558,46 +1630,52 @@
       </c>
       <c r="O13" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Ready",</v>
       </c>
       <c r="P13" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Energized"</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": -1,</v>
+        <v>"positivity": 1,</v>
       </c>
       <c r="T13" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -1605,15 +1683,15 @@
       </c>
       <c r="K14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Confused",</v>
+        <v>"name": "Jealous",</v>
       </c>
       <c r="L14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Confused Face",</v>
+        <v>"description": "Smirking Face",</v>
       </c>
       <c r="M14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😕"] ,</v>
+        <v>"characterCodes": ["😏"] ,</v>
       </c>
       <c r="N14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1621,18 +1699,18 @@
       </c>
       <c r="O14" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Envy",</v>
       </c>
       <c r="P14" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Envious"</v>
       </c>
       <c r="Q14" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S14" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1643,27 +1721,24 @@
         <v>"active": true</v>
       </c>
       <c r="U14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G15" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -1671,15 +1746,15 @@
       </c>
       <c r="K15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Disappointed, Discouraged",</v>
+        <v>"name": "Ambivalent, Neutral",</v>
       </c>
       <c r="L15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Disappointed Face",</v>
+        <v>"description": "Face with Straight Mouth",</v>
       </c>
       <c r="M15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😞"] ,</v>
+        <v>"characterCodes": ["😐"] ,</v>
       </c>
       <c r="N15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1687,7 +1762,7 @@
       </c>
       <c r="O15" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Disappointment"</v>
+        <v/>
       </c>
       <c r="P15" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1698,38 +1773,35 @@
         <v/>
       </c>
       <c r="R15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": -1,</v>
+        <v>"positivity": 0,</v>
       </c>
       <c r="T15" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1">
         <v>-1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -1737,15 +1809,15 @@
       </c>
       <c r="K16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Tense, Nervous, Anxious",</v>
+        <v>"name": "Aversion, Disgust",</v>
       </c>
       <c r="L16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Worried Face",</v>
+        <v>"description": "Unamused Face",</v>
       </c>
       <c r="M16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😟"] ,</v>
+        <v>"characterCodes": ["😒"] ,</v>
       </c>
       <c r="N16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1753,7 +1825,7 @@
       </c>
       <c r="O16" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Anxiety"</v>
+        <v/>
       </c>
       <c r="P16" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1764,7 +1836,7 @@
         <v/>
       </c>
       <c r="R16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S16" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1775,27 +1847,24 @@
         <v>"active": true</v>
       </c>
       <c r="U16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1">
         <v>-1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -1803,15 +1872,15 @@
       </c>
       <c r="K17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Furious, Outraged",</v>
+        <v>"name": "Restless, Upset",</v>
       </c>
       <c r="L17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Pouting Face",</v>
+        <v>"description": "Downcast Face with Sweat",</v>
       </c>
       <c r="M17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😡"] ,</v>
+        <v>"characterCodes": ["😓"] ,</v>
       </c>
       <c r="N17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1819,7 +1888,7 @@
       </c>
       <c r="O17" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Boiling"</v>
+        <v/>
       </c>
       <c r="P17" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1830,7 +1899,7 @@
         <v/>
       </c>
       <c r="R17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S17" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1841,24 +1910,27 @@
         <v>"active": true</v>
       </c>
       <c r="U17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
       </c>
       <c r="G18" s="1">
         <v>-1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -1866,15 +1938,15 @@
       </c>
       <c r="K18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Annoyed, Frustrated",</v>
+        <v>"name": "Confused",</v>
       </c>
       <c r="L18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Face with Steam From Nose",</v>
+        <v>"description": "Confused Face",</v>
       </c>
       <c r="M18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😤"] ,</v>
+        <v>"characterCodes": ["😕"] ,</v>
       </c>
       <c r="N18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1882,7 +1954,7 @@
       </c>
       <c r="O18" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Confusion"</v>
       </c>
       <c r="P18" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1893,7 +1965,7 @@
         <v/>
       </c>
       <c r="R18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S18" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -1904,24 +1976,27 @@
         <v>"active": true</v>
       </c>
       <c r="U18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -1929,15 +2004,15 @@
       </c>
       <c r="K19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Fatigued, Burned-Out",</v>
+        <v>"name": "Disappointed, Discouraged",</v>
       </c>
       <c r="L19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Sleepy Face",</v>
+        <v>"description": "Disappointed Face",</v>
       </c>
       <c r="M19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😪"] ,</v>
+        <v>"characterCodes": ["😞"] ,</v>
       </c>
       <c r="N19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -1945,7 +2020,7 @@
       </c>
       <c r="O19" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Disappointment"</v>
       </c>
       <c r="P19" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -1956,38 +2031,38 @@
         <v/>
       </c>
       <c r="R19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 0,</v>
+        <v>"positivity": -1,</v>
       </c>
       <c r="T19" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G20" s="1">
         <v>-1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -1995,15 +2070,15 @@
       </c>
       <c r="K20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Embarrassed, Ashamed",</v>
+        <v>"name": "Tense, Nervous, Anxious",</v>
       </c>
       <c r="L20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Grimacing Face",</v>
+        <v>"description": "Worried Face",</v>
       </c>
       <c r="M20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😬"] ,</v>
+        <v>"characterCodes": ["😟"] ,</v>
       </c>
       <c r="N20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2011,7 +2086,7 @@
       </c>
       <c r="O20" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Awkwardness"</v>
+        <v>"Anxiety"</v>
       </c>
       <c r="P20" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -2022,7 +2097,7 @@
         <v/>
       </c>
       <c r="R20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S20" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2033,27 +2108,30 @@
         <v>"active": true</v>
       </c>
       <c r="U20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>115</v>
       </c>
       <c r="G21" s="1">
         <v>-1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -2061,15 +2139,15 @@
       </c>
       <c r="K21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Afraid",</v>
+        <v>"name": "Furious, Outraged",</v>
       </c>
       <c r="L21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Anxious Face with Sweat",</v>
+        <v>"description": "Pouting Face",</v>
       </c>
       <c r="M21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["😰"] ,</v>
+        <v>"characterCodes": ["😡"] ,</v>
       </c>
       <c r="N21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2077,18 +2155,18 @@
       </c>
       <c r="O21" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Fear"</v>
+        <v>"Boiling",</v>
       </c>
       <c r="P21" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Angry"</v>
       </c>
       <c r="Q21" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S21" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2099,30 +2177,24 @@
         <v>"active": true</v>
       </c>
       <c r="U21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -2130,15 +2202,15 @@
       </c>
       <c r="K22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Calm, Relaxed",</v>
+        <v>"name": "Annoyed, Frustrated",</v>
       </c>
       <c r="L22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Slightly Smiling Face",</v>
+        <v>"description": "Face with Steam From Nose",</v>
       </c>
       <c r="M22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["🙂"] ,</v>
+        <v>"characterCodes": ["😤"] ,</v>
       </c>
       <c r="N22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2146,55 +2218,52 @@
       </c>
       <c r="O22" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Peacefulness",</v>
+        <v/>
       </c>
       <c r="P22" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v>"Serenity"</v>
+        <v/>
       </c>
       <c r="Q22" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
         <v/>
       </c>
       <c r="R22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 1,</v>
+        <v>"positivity": -1,</v>
       </c>
       <c r="T22" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -2202,15 +2271,15 @@
       </c>
       <c r="K23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Admiration",</v>
+        <v>"name": "Fatigued, Burned-Out",</v>
       </c>
       <c r="L23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Star-Struck",</v>
+        <v>"description": "Sleepy Face",</v>
       </c>
       <c r="M23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["🤩"] ,</v>
+        <v>"characterCodes": ["😪"] ,</v>
       </c>
       <c r="N23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2218,46 +2287,49 @@
       </c>
       <c r="O23" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v>"Impressed",</v>
+        <v>"Exhausted",</v>
       </c>
       <c r="P23" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
-        <v>"Pride",</v>
+        <v>"Exhaustion"</v>
       </c>
       <c r="Q23" t="str">
         <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
-        <v>"Amazement"</v>
+        <v/>
       </c>
       <c r="R23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 1,</v>
+        <v>"positivity": -1,</v>
       </c>
       <c r="T23" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
       </c>
       <c r="G24" s="1">
         <v>-1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -2265,15 +2337,15 @@
       </c>
       <c r="K24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Bored, Detached",</v>
+        <v>"name": "Embarrassed, Ashamed",</v>
       </c>
       <c r="L24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Yawning Face",</v>
+        <v>"description": "Grimacing Face",</v>
       </c>
       <c r="M24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["🥱"] ,</v>
+        <v>"characterCodes": ["😬"] ,</v>
       </c>
       <c r="N24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2281,7 +2353,7 @@
       </c>
       <c r="O24" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Awkwardness"</v>
       </c>
       <c r="P24" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -2292,7 +2364,7 @@
         <v/>
       </c>
       <c r="R24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S24" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
@@ -2303,24 +2375,27 @@
         <v>"active": true</v>
       </c>
       <c r="U24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -2328,15 +2403,15 @@
       </c>
       <c r="K25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
-        <v>"name": "Grateful, Thankful",</v>
+        <v>"name": "Afraid",</v>
       </c>
       <c r="L25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
-        <v>"description": "Partying Face",</v>
+        <v>"description": "Anxious Face with Sweat",</v>
       </c>
       <c r="M25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
-        <v>"characterCodes": ["🥳"] ,</v>
+        <v>"characterCodes": ["😰"] ,</v>
       </c>
       <c r="N25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
@@ -2344,7 +2419,7 @@
       </c>
       <c r="O25" t="str">
         <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
-        <v/>
+        <v>"Fear"</v>
       </c>
       <c r="P25" t="str">
         <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
@@ -2355,23 +2430,101 @@
         <v/>
       </c>
       <c r="R25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
-        <v>"positivity": 1,</v>
+        <v>"positivity": -1,</v>
       </c>
       <c r="T25" t="str">
         <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
         <v>"active": true</v>
       </c>
       <c r="U25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J26" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">{ </v>
+      </c>
+      <c r="K26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[name]] &amp;""": """ &amp; Table1[[#This Row],[name]] &amp; ""","</f>
+        <v>"name": "Calm, Relaxed",</v>
+      </c>
+      <c r="L26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[description]] &amp;""": """ &amp; Table1[[#This Row],[description]] &amp; ""","</f>
+        <v>"description": "Slightly Smiling Face",</v>
+      </c>
+      <c r="M26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[characterCodes]] &amp;""": [""" &amp; Table1[[#This Row],[characterCodes]] &amp; """] ,"</f>
+        <v>"characterCodes": ["🙂"] ,</v>
+      </c>
+      <c r="N26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[related]] &amp;""": ["</f>
+        <v>"related": [</v>
+      </c>
+      <c r="O26" t="str">
+        <f>IF(Table1[[#This Row],[related]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related]]&amp;"""","") &amp; IF(Table1[[#This Row],[related2]] &lt;&gt; "", ",", "")</f>
+        <v>"Peacefulness",</v>
+      </c>
+      <c r="P26" t="str">
+        <f>IF(Table1[[#This Row],[related2]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related2]]&amp;"""","") &amp; IF(Table1[[#This Row],[related3]] &lt;&gt; "", ",", "")</f>
+        <v>"Serenity"</v>
+      </c>
+      <c r="Q26" t="str">
+        <f>IF(Table1[[#This Row],[related3]]&lt;&gt;"",""""&amp;Table1[[#This Row],[related3]]&amp;"""","")</f>
+        <v/>
+      </c>
+      <c r="R26" t="s">
+        <v>94</v>
+      </c>
+      <c r="S26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[positivity]] &amp;""": " &amp; Table1[[#This Row],[positivity]] &amp; ","</f>
+        <v>"positivity": 1,</v>
+      </c>
+      <c r="T26" t="str">
+        <f xml:space="preserve"> """" &amp; Table1[[#Headers],[active]] &amp;""": " &amp; Table1[[#This Row],[active]]</f>
+        <v>"active": true</v>
+      </c>
+      <c r="U26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="G27" s="1">
+        <f>SUBTOTAL(109,Table1[positivity])</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="J27" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix account recovery page and disable logging
</commit_message>
<xml_diff>
--- a/Server/testData/rawAffects/NewAffects.xlsx
+++ b/Server/testData/rawAffects/NewAffects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berriers/Programming/eec-common-repo/Server/testData/rawAffects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming-School\eec-common-repo\Server\testData\rawAffects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970250E-15A0-5242-9204-EDF460D012FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285066D0-450B-4AF4-B3B4-D7D32B9D23FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40940" yWindow="2660" windowWidth="40960" windowHeight="22540" xr2:uid="{29D9A252-B3D8-4ABB-AC96-716C0C40817A}"/>
+    <workbookView xWindow="570" yWindow="495" windowWidth="22125" windowHeight="19935" xr2:uid="{29D9A252-B3D8-4ABB-AC96-716C0C40817A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,12 +479,12 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{937E03AA-42B8-4F21-8CED-841BB10CDD05}" name="name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F560CCD9-0FE5-4B5D-8A1D-D0BC3D9FA4E4}" name="description"/>
-    <tableColumn id="3" xr3:uid="{D1F9F36A-4F9F-43B8-B427-C52F36F043CC}" name="characterCodes" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D1F9F36A-4F9F-43B8-B427-C52F36F043CC}" name="characterCodes" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="4" xr3:uid="{744D4406-D359-409C-8C64-155246DB37C4}" name="related"/>
     <tableColumn id="8" xr3:uid="{E58DFCE5-051E-4701-B194-FEEABBB3FBC5}" name="related2"/>
     <tableColumn id="7" xr3:uid="{231F6072-1022-47BD-811D-E33DB8FEE891}" name="related3"/>
-    <tableColumn id="5" xr3:uid="{FB2190ED-A4F5-4603-A60F-8C9354525546}" name="positivity" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C044B12F-37E2-408D-A1AF-524B258708DA}" name="active" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{FB2190ED-A4F5-4603-A60F-8C9354525546}" name="positivity" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C044B12F-37E2-408D-A1AF-524B258708DA}" name="active" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -793,33 +793,33 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -920,7 +920,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -986,7 +986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>117</v>
       </c>

</xml_diff>